<commit_message>
create abstract entities for the entity element in the template
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/PhenDB/PhenDB_NMC/PhenDB_NMC.xlsx
+++ b/molgenis-model-registry/src/test/resources/PhenDB/PhenDB_NMC/PhenDB_NMC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="2380" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="223">
   <si>
     <t>name</t>
   </si>
@@ -719,6 +719,15 @@
   <si>
     <t>MB version for the Cell line use case.
 Variables in this are for the 5 markers in the kit and the overall call of microsatellite (in)stable.</t>
+  </si>
+  <si>
+    <t>org.dbxp.sam.Feature</t>
+  </si>
+  <si>
+    <t>extends</t>
+  </si>
+  <si>
+    <t>abstract</t>
   </si>
 </sst>
 </file>
@@ -1238,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G165"/>
+  <dimension ref="A1:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection sqref="A1:G165"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1273,11 +1282,8 @@
       <c r="A2" t="s">
         <v>215</v>
       </c>
-      <c r="B2" t="s">
-        <v>215</v>
-      </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1294,27 +1300,33 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
         <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>193</v>
@@ -1325,16 +1337,13 @@
       <c r="F4" t="b">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>193</v>
@@ -1346,15 +1355,15 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="75">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="90">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>193</v>
@@ -1366,15 +1375,15 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="135">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>193</v>
@@ -1386,15 +1395,15 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="135">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>193</v>
@@ -1405,56 +1414,56 @@
       <c r="F8" t="b">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
-        <v>43</v>
+      <c r="G8" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>193</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>193</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>193</v>
@@ -1466,15 +1475,15 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="120">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="150">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>193</v>
@@ -1486,15 +1495,15 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="75">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="120">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>193</v>
@@ -1506,15 +1515,15 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
         <v>193</v>
@@ -1525,76 +1534,76 @@
       <c r="F14" t="b">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
-        <v>55</v>
+      <c r="G14" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>193</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="210">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="105">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>193</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="210">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>193</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
-        <v>60</v>
+      <c r="G17" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
         <v>193</v>
@@ -1605,13 +1614,16 @@
       <c r="F18" t="b">
         <v>1</v>
       </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
         <v>193</v>
@@ -1622,36 +1634,33 @@
       <c r="F19" t="b">
         <v>1</v>
       </c>
-      <c r="G19" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
         <v>193</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
         <v>193</v>
@@ -1663,32 +1672,35 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
         <v>193</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
         <v>193</v>
@@ -1700,75 +1712,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="300">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
         <v>193</v>
       </c>
       <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="300">
+      <c r="A25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>215</v>
-      </c>
-      <c r="B25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C25" t="s">
-        <v>195</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>215</v>
       </c>
       <c r="C26" t="s">
         <v>195</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
       </c>
       <c r="F26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>73</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
         <v>195</v>
@@ -1780,38 +1790,41 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
         <v>195</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
         <v>195</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
@@ -1819,47 +1832,47 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
         <v>195</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
-      </c>
-      <c r="G30" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
         <v>195</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="b">
         <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
         <v>195</v>
@@ -1873,10 +1886,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
         <v>195</v>
@@ -1887,36 +1900,33 @@
       <c r="F33" t="b">
         <v>1</v>
       </c>
-      <c r="G33" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
         <v>195</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F34" t="b">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
         <v>195</v>
@@ -1928,15 +1938,15 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="210">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="150">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
         <v>195</v>
@@ -1948,15 +1958,15 @@
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="300">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="210">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
         <v>195</v>
@@ -1968,15 +1978,15 @@
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="300">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
         <v>195</v>
@@ -1987,16 +1997,16 @@
       <c r="F38" t="b">
         <v>1</v>
       </c>
-      <c r="G38" t="s">
-        <v>65</v>
+      <c r="G38" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
         <v>195</v>
@@ -2007,56 +2017,56 @@
       <c r="F39" t="b">
         <v>1</v>
       </c>
+      <c r="G39" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F40" t="b">
-        <v>0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>216</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>215</v>
       </c>
       <c r="C41" t="s">
         <v>198</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
       </c>
       <c r="F41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>73</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
         <v>198</v>
@@ -2068,38 +2078,41 @@
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
         <v>198</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
         <v>198</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
@@ -2107,47 +2120,47 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C45" t="s">
         <v>198</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
-      </c>
-      <c r="G45" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
         <v>198</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
         <v>198</v>
@@ -2161,10 +2174,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
         <v>198</v>
@@ -2175,36 +2188,33 @@
       <c r="F48" t="b">
         <v>1</v>
       </c>
-      <c r="G48" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
         <v>198</v>
       </c>
       <c r="D49" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
         <v>198</v>
@@ -2216,15 +2226,15 @@
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="210">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="150">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
         <v>198</v>
@@ -2236,15 +2246,15 @@
         <v>1</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="300">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="210">
       <c r="A52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
         <v>198</v>
@@ -2256,15 +2266,15 @@
         <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="300">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
         <v>198</v>
@@ -2275,16 +2285,16 @@
       <c r="F53" t="b">
         <v>1</v>
       </c>
-      <c r="G53" t="s">
-        <v>65</v>
+      <c r="G53" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
         <v>198</v>
@@ -2295,56 +2305,56 @@
       <c r="F54" t="b">
         <v>1</v>
       </c>
+      <c r="G54" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="B55" t="s">
-        <v>215</v>
+        <v>88</v>
       </c>
       <c r="C55" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" t="b">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F55" t="b">
-        <v>0</v>
-      </c>
-      <c r="G55" t="s">
-        <v>216</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="B56" t="s">
-        <v>34</v>
+        <v>215</v>
       </c>
       <c r="C56" t="s">
         <v>201</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
       </c>
       <c r="F56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="75">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="90">
       <c r="A57" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
         <v>201</v>
@@ -2356,15 +2366,15 @@
         <v>1</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="75">
       <c r="A58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C58" t="s">
         <v>201</v>
@@ -2375,16 +2385,16 @@
       <c r="F58" t="b">
         <v>1</v>
       </c>
-      <c r="G58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="150">
+      <c r="G58" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="90">
       <c r="A59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
         <v>201</v>
@@ -2396,15 +2406,15 @@
         <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="135">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="150">
       <c r="A60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C60" t="s">
         <v>201</v>
@@ -2416,15 +2426,15 @@
         <v>1</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="165">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="135">
       <c r="A61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B61" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C61" t="s">
         <v>201</v>
@@ -2436,15 +2446,15 @@
         <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="135">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="165">
       <c r="A62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C62" t="s">
         <v>201</v>
@@ -2456,15 +2466,15 @@
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="135">
       <c r="A63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B63" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C63" t="s">
         <v>201</v>
@@ -2476,15 +2486,15 @@
         <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="165">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="135">
       <c r="A64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C64" t="s">
         <v>201</v>
@@ -2496,15 +2506,15 @@
         <v>1</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="135">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="165">
       <c r="A65" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B65" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
         <v>201</v>
@@ -2516,95 +2526,95 @@
         <v>1</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="135">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C66" t="s">
         <v>201</v>
       </c>
       <c r="D66" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="F66" t="b">
         <v>1</v>
       </c>
-      <c r="G66" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="150">
+      <c r="G66" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="180">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
         <v>201</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="F67" t="b">
         <v>1</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="150">
       <c r="A68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C68" t="s">
         <v>201</v>
       </c>
       <c r="D68" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="F68" t="b">
         <v>1</v>
       </c>
-      <c r="G68" t="s">
-        <v>108</v>
+      <c r="G68" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="C69" t="s">
         <v>201</v>
       </c>
       <c r="D69" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="F69" t="b">
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="120">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="150">
       <c r="A70" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C70" t="s">
         <v>201</v>
@@ -2616,15 +2626,15 @@
         <v>1</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="120">
       <c r="A71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B71" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C71" t="s">
         <v>201</v>
@@ -2635,16 +2645,16 @@
       <c r="F71" t="b">
         <v>1</v>
       </c>
-      <c r="G71" t="s">
-        <v>49</v>
+      <c r="G71" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="150">
       <c r="A72" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B72" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="C72" t="s">
         <v>201</v>
@@ -2656,15 +2666,15 @@
         <v>1</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="150">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C73" t="s">
         <v>201</v>
@@ -2676,15 +2686,15 @@
         <v>1</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="150">
       <c r="A74" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B74" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C74" t="s">
         <v>201</v>
@@ -2696,15 +2706,15 @@
         <v>1</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="150">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B75" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C75" t="s">
         <v>201</v>
@@ -2716,15 +2726,15 @@
         <v>1</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="120">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="150">
       <c r="A76" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C76" t="s">
         <v>201</v>
@@ -2736,15 +2746,15 @@
         <v>1</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="150">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="120">
       <c r="A77" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C77" t="s">
         <v>201</v>
@@ -2756,35 +2766,35 @@
         <v>1</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="150">
       <c r="A78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B78" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="C78" t="s">
         <v>201</v>
       </c>
       <c r="D78" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F78" t="b">
         <v>1</v>
       </c>
-      <c r="G78" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="210">
+      <c r="G78" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="180">
       <c r="A79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C79" t="s">
         <v>201</v>
@@ -2796,15 +2806,15 @@
         <v>1</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="210">
       <c r="A80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="C80" t="s">
         <v>201</v>
@@ -2815,19 +2825,22 @@
       <c r="F80" t="b">
         <v>1</v>
       </c>
+      <c r="G80" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C81" t="s">
         <v>201</v>
       </c>
       <c r="D81" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F81" t="b">
         <v>1</v>
@@ -2835,10 +2848,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B82" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="C82" t="s">
         <v>201</v>
@@ -2849,59 +2862,56 @@
       <c r="F82" t="b">
         <v>1</v>
       </c>
-      <c r="G82" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="B83" t="s">
-        <v>215</v>
+        <v>121</v>
       </c>
       <c r="C83" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D83" t="s">
-        <v>6</v>
-      </c>
-      <c r="E83" t="b">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>216</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="B84" t="s">
-        <v>36</v>
+        <v>215</v>
       </c>
       <c r="C84" t="s">
         <v>203</v>
       </c>
       <c r="D84" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
       </c>
       <c r="F84" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G84" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B85" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C85" t="s">
         <v>203</v>
@@ -2912,13 +2922,16 @@
       <c r="F85" t="b">
         <v>1</v>
       </c>
+      <c r="G85" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="C86" t="s">
         <v>203</v>
@@ -2929,16 +2942,13 @@
       <c r="F86" t="b">
         <v>1</v>
       </c>
-      <c r="G86" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="135">
+    </row>
+    <row r="87" spans="1:7" ht="45">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B87" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="C87" t="s">
         <v>203</v>
@@ -2950,135 +2960,135 @@
         <v>1</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="135">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B88" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C88" t="s">
         <v>203</v>
       </c>
       <c r="D88" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="F88" t="b">
         <v>1</v>
       </c>
-      <c r="G88" t="s">
-        <v>45</v>
+      <c r="G88" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C89" t="s">
         <v>203</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="F89" t="b">
         <v>1</v>
       </c>
       <c r="G89" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="75">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="90">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="C90" t="s">
         <v>203</v>
       </c>
       <c r="D90" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F90" t="b">
         <v>1</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="75">
       <c r="A91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B91" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C91" t="s">
         <v>203</v>
       </c>
       <c r="D91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="b">
         <v>1</v>
       </c>
-      <c r="G91" t="s">
-        <v>128</v>
+      <c r="G91" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B92" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C92" t="s">
         <v>203</v>
       </c>
       <c r="D92" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F92" t="b">
         <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="300">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="60">
       <c r="A93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="C93" t="s">
         <v>203</v>
       </c>
       <c r="D93" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F93" t="b">
         <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="210">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="300">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C94" t="s">
         <v>203</v>
@@ -3090,15 +3100,15 @@
         <v>1</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="210">
       <c r="A95" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B95" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="C95" t="s">
         <v>203</v>
@@ -3109,19 +3119,22 @@
       <c r="F95" t="b">
         <v>1</v>
       </c>
+      <c r="G95" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C96" t="s">
         <v>203</v>
       </c>
       <c r="D96" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F96" t="b">
         <v>1</v>
@@ -3129,10 +3142,10 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C97" t="s">
         <v>203</v>
@@ -3143,76 +3156,74 @@
       <c r="F97" t="b">
         <v>1</v>
       </c>
-      <c r="G97" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>215</v>
+        <v>82</v>
       </c>
       <c r="C98" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98" t="b">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>216</v>
+        <v>83</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>215</v>
       </c>
       <c r="C99" t="s">
         <v>206</v>
       </c>
       <c r="D99" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
       </c>
       <c r="F99" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="120">
+        <v>0</v>
+      </c>
+      <c r="G99" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B100" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C100" t="s">
         <v>206</v>
       </c>
       <c r="D100" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F100" t="b">
         <v>1</v>
       </c>
-      <c r="G100" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="150">
+      <c r="G100" s="2"/>
+    </row>
+    <row r="101" spans="1:7" ht="120">
       <c r="A101" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B101" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C101" t="s">
         <v>206</v>
@@ -3224,15 +3235,15 @@
         <v>1</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="165">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="150">
       <c r="A102" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B102" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C102" t="s">
         <v>206</v>
@@ -3244,15 +3255,15 @@
         <v>1</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="180">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="165">
       <c r="A103" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B103" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C103" t="s">
         <v>206</v>
@@ -3264,112 +3275,113 @@
         <v>1</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="150">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="180">
       <c r="A104" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B104" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C104" t="s">
         <v>206</v>
       </c>
       <c r="D104" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F104" t="b">
         <v>1</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="165">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="150">
       <c r="A105" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B105" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C105" t="s">
         <v>206</v>
       </c>
       <c r="D105" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F105" t="b">
         <v>1</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="165">
       <c r="A106" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B106" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C106" t="s">
         <v>206</v>
       </c>
       <c r="D106" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F106" t="b">
         <v>1</v>
       </c>
-      <c r="G106" t="s">
-        <v>145</v>
+      <c r="G106" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B107" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="C107" t="s">
         <v>206</v>
       </c>
       <c r="D107" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F107" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="300">
+      <c r="G107" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B108" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C108" t="s">
         <v>206</v>
       </c>
       <c r="D108" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F108" t="b">
         <v>1</v>
       </c>
-      <c r="G108" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="210">
+      <c r="G108" s="2"/>
+    </row>
+    <row r="109" spans="1:7" ht="300">
       <c r="A109" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B109" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C109" t="s">
         <v>206</v>
@@ -3381,15 +3393,15 @@
         <v>1</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="210">
       <c r="A110" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B110" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
       <c r="C110" t="s">
         <v>206</v>
@@ -3400,16 +3412,16 @@
       <c r="F110" t="b">
         <v>1</v>
       </c>
-      <c r="G110" t="s">
-        <v>147</v>
+      <c r="G110" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B111" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C111" t="s">
         <v>206</v>
@@ -3421,58 +3433,58 @@
         <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="B112" t="s">
-        <v>215</v>
+        <v>148</v>
       </c>
       <c r="C112" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D112" t="s">
-        <v>6</v>
-      </c>
-      <c r="E112" t="b">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G112" t="s">
-        <v>216</v>
+        <v>149</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="B113" t="s">
-        <v>36</v>
+        <v>215</v>
       </c>
       <c r="C113" t="s">
         <v>208</v>
       </c>
       <c r="D113" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E113" t="b">
+        <v>1</v>
       </c>
       <c r="F113" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B114" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C114" t="s">
         <v>208</v>
@@ -3483,13 +3495,16 @@
       <c r="F114" t="b">
         <v>1</v>
       </c>
+      <c r="G114" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B115" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="C115" t="s">
         <v>208</v>
@@ -3500,16 +3515,13 @@
       <c r="F115" t="b">
         <v>1</v>
       </c>
-      <c r="G115" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="135">
+    </row>
+    <row r="116" spans="1:7" ht="45">
       <c r="A116" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B116" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="C116" t="s">
         <v>208</v>
@@ -3521,15 +3533,15 @@
         <v>1</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="135">
       <c r="A117" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B117" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C117" t="s">
         <v>208</v>
@@ -3540,56 +3552,56 @@
       <c r="F117" t="b">
         <v>1</v>
       </c>
-      <c r="G117" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="75">
+      <c r="G117" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="90">
       <c r="A118" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B118" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="C118" t="s">
         <v>208</v>
       </c>
       <c r="D118" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F118" t="b">
         <v>1</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="75">
       <c r="A119" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B119" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C119" t="s">
         <v>208</v>
       </c>
       <c r="D119" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F119" t="b">
         <v>1</v>
       </c>
-      <c r="G119" t="s">
-        <v>128</v>
+      <c r="G119" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B120" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="C120" t="s">
         <v>208</v>
@@ -3600,33 +3612,33 @@
       <c r="F120" t="b">
         <v>1</v>
       </c>
+      <c r="G120" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B121" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="C121" t="s">
         <v>208</v>
       </c>
       <c r="D121" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F121" t="b">
         <v>1</v>
       </c>
-      <c r="G121" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="135">
+    </row>
+    <row r="122" spans="1:7" ht="60">
       <c r="A122" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B122" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="C122" t="s">
         <v>208</v>
@@ -3638,35 +3650,35 @@
         <v>1</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="300">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="135">
       <c r="A123" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B123" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="C123" t="s">
         <v>208</v>
       </c>
       <c r="D123" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F123" t="b">
         <v>1</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="210">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="300">
       <c r="A124" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B124" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C124" t="s">
         <v>208</v>
@@ -3678,15 +3690,15 @@
         <v>1</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="210">
       <c r="A125" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B125" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="C125" t="s">
         <v>208</v>
@@ -3697,19 +3709,22 @@
       <c r="F125" t="b">
         <v>1</v>
       </c>
+      <c r="G125" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B126" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C126" t="s">
         <v>208</v>
       </c>
       <c r="D126" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F126" t="b">
         <v>1</v>
@@ -3717,10 +3732,10 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B127" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C127" t="s">
         <v>208</v>
@@ -3731,56 +3746,56 @@
       <c r="F127" t="b">
         <v>1</v>
       </c>
-      <c r="G127" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="B128" t="s">
-        <v>215</v>
+        <v>82</v>
       </c>
       <c r="C128" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D128" t="s">
-        <v>6</v>
-      </c>
-      <c r="E128" t="b">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F128" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G128" t="s">
-        <v>216</v>
+        <v>83</v>
       </c>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="B129" t="s">
-        <v>33</v>
+        <v>215</v>
       </c>
       <c r="C129" t="s">
         <v>211</v>
       </c>
       <c r="D129" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E129" t="b">
+        <v>1</v>
       </c>
       <c r="F129" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G129" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B130" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C130" t="s">
         <v>211</v>
@@ -3791,16 +3806,13 @@
       <c r="F130" t="b">
         <v>1</v>
       </c>
-      <c r="G130" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B131" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C131" t="s">
         <v>211</v>
@@ -3812,15 +3824,15 @@
         <v>1</v>
       </c>
       <c r="G131" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" ht="75">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="90">
       <c r="A132" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B132" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C132" t="s">
         <v>211</v>
@@ -3832,15 +3844,15 @@
         <v>1</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" ht="135">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="75">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B133" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C133" t="s">
         <v>211</v>
@@ -3852,15 +3864,15 @@
         <v>1</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="135">
       <c r="A134" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B134" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C134" t="s">
         <v>211</v>
@@ -3871,16 +3883,16 @@
       <c r="F134" t="b">
         <v>1</v>
       </c>
-      <c r="G134" t="s">
-        <v>43</v>
+      <c r="G134" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B135" t="s">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="C135" t="s">
         <v>211</v>
@@ -3892,55 +3904,55 @@
         <v>1</v>
       </c>
       <c r="G135" t="s">
-        <v>154</v>
+        <v>43</v>
       </c>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B136" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="C136" t="s">
         <v>211</v>
       </c>
       <c r="D136" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="F136" t="b">
         <v>1</v>
       </c>
       <c r="G136" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B137" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C137" t="s">
         <v>211</v>
       </c>
       <c r="D137" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="F137" t="b">
         <v>1</v>
       </c>
       <c r="G137" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="138" spans="1:7">
       <c r="A138" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B138" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C138" t="s">
         <v>211</v>
@@ -3952,15 +3964,15 @@
         <v>1</v>
       </c>
       <c r="G138" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="120">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="150">
       <c r="A139" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B139" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C139" t="s">
         <v>211</v>
@@ -3972,15 +3984,15 @@
         <v>1</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" ht="75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="120">
       <c r="A140" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B140" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C140" t="s">
         <v>211</v>
@@ -3992,15 +4004,15 @@
         <v>1</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="75">
       <c r="A141" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B141" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C141" t="s">
         <v>211</v>
@@ -4011,16 +4023,16 @@
       <c r="F141" t="b">
         <v>1</v>
       </c>
-      <c r="G141" t="s">
-        <v>55</v>
+      <c r="G141" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B142" t="s">
-        <v>155</v>
+        <v>54</v>
       </c>
       <c r="C142" t="s">
         <v>211</v>
@@ -4032,92 +4044,92 @@
         <v>1</v>
       </c>
       <c r="G142" t="s">
-        <v>156</v>
+        <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B143" t="s">
-        <v>56</v>
+        <v>155</v>
       </c>
       <c r="C143" t="s">
         <v>211</v>
       </c>
       <c r="D143" t="s">
-        <v>163</v>
+        <v>8</v>
       </c>
       <c r="F143" t="b">
         <v>1</v>
       </c>
       <c r="G143" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="210">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="105">
       <c r="A144" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B144" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C144" t="s">
         <v>211</v>
       </c>
       <c r="D144" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="F144" t="b">
         <v>1</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="210">
       <c r="A145" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B145" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C145" t="s">
         <v>211</v>
       </c>
       <c r="D145" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F145" t="b">
         <v>1</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="146" spans="1:7">
       <c r="A146" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B146" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C146" t="s">
         <v>211</v>
       </c>
       <c r="D146" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F146" t="b">
         <v>1</v>
-      </c>
-      <c r="G146" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="147" spans="1:7">
       <c r="A147" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B147" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C147" t="s">
         <v>211</v>
@@ -4129,32 +4141,35 @@
         <v>1</v>
       </c>
       <c r="G147" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="148" spans="1:7">
       <c r="A148" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B148" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C148" t="s">
         <v>211</v>
       </c>
       <c r="D148" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F148" t="b">
         <v>1</v>
+      </c>
+      <c r="G148" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B149" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C149" t="s">
         <v>211</v>
@@ -4166,112 +4181,113 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="300">
+    <row r="150" spans="1:7">
       <c r="A150" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B150" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C150" t="s">
         <v>211</v>
       </c>
       <c r="D150" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F150" t="b">
         <v>1</v>
       </c>
-      <c r="G150" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7">
+      <c r="G150" s="2"/>
+    </row>
+    <row r="151" spans="1:7" ht="300">
       <c r="A151" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B151" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="C151" t="s">
         <v>211</v>
       </c>
       <c r="D151" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F151" t="b">
         <v>1</v>
       </c>
-      <c r="G151" t="s">
-        <v>122</v>
+      <c r="G151" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="152" spans="1:7">
       <c r="A152" t="s">
+        <v>186</v>
+      </c>
+      <c r="B152" t="s">
+        <v>121</v>
+      </c>
+      <c r="C152" t="s">
+        <v>211</v>
+      </c>
+      <c r="D152" t="s">
+        <v>8</v>
+      </c>
+      <c r="F152" t="b">
+        <v>1</v>
+      </c>
+      <c r="G152" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="30">
+      <c r="A153" t="s">
         <v>215</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B153" t="s">
         <v>215</v>
-      </c>
-      <c r="C152" t="s">
-        <v>213</v>
-      </c>
-      <c r="D152" t="s">
-        <v>6</v>
-      </c>
-      <c r="E152" t="b">
-        <v>1</v>
-      </c>
-      <c r="F152" t="b">
-        <v>0</v>
-      </c>
-      <c r="G152" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" ht="195">
-      <c r="A153" t="s">
-        <v>164</v>
-      </c>
-      <c r="B153" t="s">
-        <v>157</v>
       </c>
       <c r="C153" t="s">
         <v>213</v>
       </c>
       <c r="D153" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E153" t="b">
+        <v>1</v>
       </c>
       <c r="F153" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="195">
       <c r="A154" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B154" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="C154" t="s">
         <v>213</v>
       </c>
       <c r="D154" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F154" t="b">
         <v>1</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="155" spans="1:7">
       <c r="A155" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B155" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C155" t="s">
         <v>213</v>
@@ -4282,16 +4298,13 @@
       <c r="F155" t="b">
         <v>1</v>
       </c>
-      <c r="G155" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="156" spans="1:7">
       <c r="A156" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B156" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="C156" t="s">
         <v>213</v>
@@ -4303,15 +4316,15 @@
         <v>1</v>
       </c>
       <c r="G156" t="s">
-        <v>124</v>
+        <v>37</v>
       </c>
     </row>
     <row r="157" spans="1:7">
       <c r="A157" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B157" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C157" t="s">
         <v>213</v>
@@ -4323,132 +4336,133 @@
         <v>1</v>
       </c>
       <c r="G157" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" ht="75">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="45">
       <c r="A158" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B158" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C158" t="s">
         <v>213</v>
       </c>
       <c r="D158" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F158" t="b">
         <v>1</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="75">
       <c r="A159" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B159" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="C159" t="s">
         <v>213</v>
       </c>
       <c r="D159" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F159" t="b">
         <v>1</v>
       </c>
-      <c r="G159" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" ht="105">
+      <c r="G159" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="90">
       <c r="A160" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B160" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C160" t="s">
         <v>213</v>
       </c>
       <c r="D160" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F160" t="b">
         <v>1</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" ht="210">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="105">
       <c r="A161" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B161" t="s">
-        <v>12</v>
+        <v>160</v>
       </c>
       <c r="C161" t="s">
         <v>213</v>
       </c>
       <c r="D161" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F161" t="b">
         <v>1</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="210">
       <c r="A162" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B162" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="C162" t="s">
         <v>213</v>
       </c>
       <c r="D162" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F162" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" ht="300">
+      <c r="G162" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
       <c r="A163" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B163" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C163" t="s">
         <v>213</v>
       </c>
       <c r="D163" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F163" t="b">
         <v>1</v>
       </c>
-      <c r="G163" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7">
+      <c r="G163" s="2"/>
+    </row>
+    <row r="164" spans="1:7" ht="300">
       <c r="A164" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B164" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C164" t="s">
         <v>213</v>
@@ -4459,21 +4473,41 @@
       <c r="F164" t="b">
         <v>1</v>
       </c>
+      <c r="G164" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="165" spans="1:7">
       <c r="A165" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B165" t="s">
-        <v>162</v>
+        <v>88</v>
       </c>
       <c r="C165" t="s">
         <v>213</v>
       </c>
       <c r="D165" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F165" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" t="s">
+        <v>176</v>
+      </c>
+      <c r="B166" t="s">
+        <v>162</v>
+      </c>
+      <c r="C166" t="s">
+        <v>213</v>
+      </c>
+      <c r="D166" t="s">
+        <v>8</v>
+      </c>
+      <c r="F166" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4490,10 +4524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4502,7 +4536,7 @@
     <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4513,129 +4547,202 @@
         <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>221</v>
+      </c>
+      <c r="E1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>220</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>220</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="210">
+        <v>220</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>220</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="210">
       <c r="A8" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>220</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>220</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>217</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" t="s">
         <v>214</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>